<commit_message>
modify the field of bloomberg data
</commit_message>
<xml_diff>
--- a/strategy/output.xlsx
+++ b/strategy/output.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Konan/Desktop/github/financialUtility/strategy/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="620" windowWidth="25360" windowHeight="15380"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="150001" iterate="1" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
-  <si>
-    <t xml:space="preserve">BEst NI:2016C
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">NI / Profit:2016C
 </t>
   </si>
   <si>
@@ -35,27 +48,24 @@
     <t>remark</t>
   </si>
   <si>
-    <t>NDX INDEX</t>
+    <t>SPX INDEX</t>
   </si>
   <si>
     <t>剔除0家</t>
   </si>
   <si>
-    <t>SPX INDEX</t>
+    <t>DJI INDEX</t>
+  </si>
+  <si>
+    <t>SX5E INDEX</t>
+  </si>
+  <si>
+    <t>UKX INDEX</t>
   </si>
   <si>
     <t>剔除1家</t>
   </si>
   <si>
-    <t>DJI INDEX</t>
-  </si>
-  <si>
-    <t>SX5E INDEX</t>
-  </si>
-  <si>
-    <t>UKX INDEX</t>
-  </si>
-  <si>
     <t>CAC INDEX</t>
   </si>
   <si>
@@ -65,7 +75,7 @@
     <t>NKY INDEX</t>
   </si>
   <si>
-    <t>剔除6家</t>
+    <t>剔除5家</t>
   </si>
   <si>
     <t>HSI INDEX</t>
@@ -74,29 +84,38 @@
     <t>KOSPI2 INDEX</t>
   </si>
   <si>
-    <t>剔除45家</t>
+    <t>剔除40家</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -111,26 +130,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -418,20 +451,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,207 +483,188 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>315511044433.3586</v>
-      </c>
-      <c r="C2" t="n">
-        <v>369459701468.0923</v>
-      </c>
-      <c r="D2" t="n">
-        <v>440522718917.1987</v>
-      </c>
-      <c r="E2" t="n">
-        <v>8697168565248</v>
+      <c r="B2">
+        <v>9455</v>
+      </c>
+      <c r="C2">
+        <v>12201</v>
+      </c>
+      <c r="D2">
+        <v>14456</v>
+      </c>
+      <c r="E2">
+        <v>247426</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="n">
-        <v>1094455278464</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1217637907924</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1442946822210</v>
-      </c>
-      <c r="E3" t="n">
-        <v>24710003453440</v>
+      <c r="B3">
+        <v>2857</v>
+      </c>
+      <c r="C3">
+        <v>3512</v>
+      </c>
+      <c r="D3">
+        <v>4081</v>
+      </c>
+      <c r="E3">
+        <v>66393</v>
       </c>
       <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="n">
-        <v>322362929024</v>
-      </c>
-      <c r="C4" t="n">
-        <v>351235203584</v>
-      </c>
-      <c r="D4" t="n">
-        <v>408126472704</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6639329882112</v>
+      <c r="B4">
+        <v>1515.8075285649279</v>
+      </c>
+      <c r="C4">
+        <v>2302.6403022893342</v>
+      </c>
+      <c r="D4">
+        <v>2586.754283448457</v>
+      </c>
+      <c r="E4">
+        <v>35975.383969014598</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>821.77335431575227</v>
+      </c>
+      <c r="C5">
+        <v>2085.268417675537</v>
+      </c>
+      <c r="D5">
+        <v>2397.9354197345001</v>
+      </c>
+      <c r="E5">
+        <v>32571.225171214501</v>
+      </c>
+      <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="n">
-        <v>184047130618.5921</v>
-      </c>
-      <c r="C5" t="n">
-        <v>230264030228.9334</v>
-      </c>
-      <c r="D5" t="n">
-        <v>258675428344.8456</v>
-      </c>
-      <c r="E5" t="n">
-        <v>3587032074897.501</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="n">
-        <v>152750236166.4383</v>
-      </c>
-      <c r="C6" t="n">
-        <v>208526841767.5537</v>
-      </c>
-      <c r="D6" t="n">
-        <v>239851541333.45</v>
-      </c>
-      <c r="E6" t="n">
-        <v>3257122517121.45</v>
+      <c r="B6">
+        <v>840.2465927390009</v>
+      </c>
+      <c r="C6">
+        <v>1119.717264051656</v>
+      </c>
+      <c r="D6">
+        <v>1237.030531556084</v>
+      </c>
+      <c r="E6">
+        <v>18050.884119603641</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="n">
-        <v>87836417143.3317</v>
-      </c>
-      <c r="C7" t="n">
-        <v>111971726405.1656</v>
-      </c>
-      <c r="D7" t="n">
-        <v>123703053155.6084</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1805088411960.364</v>
+      <c r="B7">
+        <v>642.19006670598208</v>
+      </c>
+      <c r="C7">
+        <v>1131.2116797746089</v>
+      </c>
+      <c r="D7">
+        <v>1262.0500083690081</v>
+      </c>
+      <c r="E7">
+        <v>15382.08671252362</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="n">
-        <v>90748031011.23341</v>
-      </c>
-      <c r="C8" t="n">
-        <v>111399220791.7426</v>
-      </c>
-      <c r="D8" t="n">
-        <v>124293248502.2902</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1499234863415.323</v>
+      <c r="B8">
+        <v>1719.968160995759</v>
+      </c>
+      <c r="C8">
+        <v>2041.6904518692891</v>
+      </c>
+      <c r="D8">
+        <v>2741.4681304007322</v>
+      </c>
+      <c r="E8">
+        <v>35361.039022053948</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="n">
-        <v>189313376546.3425</v>
-      </c>
-      <c r="C9" t="n">
-        <v>205024347854.9032</v>
-      </c>
-      <c r="D9" t="n">
-        <v>274578821329.0187</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3527273780953.92</v>
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>2249.6241580719361</v>
+      </c>
+      <c r="C9">
+        <v>2593.689219144082</v>
+      </c>
+      <c r="D9">
+        <v>3056.3380952640832</v>
+      </c>
+      <c r="E9">
+        <v>34943.296163098094</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="n">
-        <v>216917864562.1722</v>
-      </c>
-      <c r="C10" t="n">
-        <v>259368921914.4083</v>
-      </c>
-      <c r="D10" t="n">
-        <v>305734771029.2366</v>
-      </c>
-      <c r="E10" t="n">
-        <v>3494329616309.809</v>
+      <c r="B10">
+        <v>783.78104572736379</v>
+      </c>
+      <c r="C10">
+        <v>1230.0102538315521</v>
+      </c>
+      <c r="D10">
+        <v>1363.32906124335</v>
+      </c>
+      <c r="E10">
+        <v>12740.618683542891</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="n">
-        <v>80525016877.23705</v>
-      </c>
-      <c r="C11" t="n">
-        <v>122760087854.3566</v>
-      </c>
-      <c r="D11" t="n">
-        <v>135615121270.319</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1268801660719.762</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>